<commit_message>
data: replication files for slr and gray lit rev
</commit_message>
<xml_diff>
--- a/multivocal_literature_review/gray_literature_review.xlsx
+++ b/multivocal_literature_review/gray_literature_review.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simon/Documents/Own/Papers_and_Projects/comparison_ArchRec_tools/GitHub_SARbenchmarks/multivocal_literature_review/gray_literature_review/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simon/Documents/Own/Papers_and_Projects/comparison_ArchRec_tools/GitHub_SARbenchmarks/multivocal_literature_review/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79EDAFCB-2270-1A4D-BB4D-2D15297290F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4F85B5-F6FF-E14B-860C-E5A43985E3A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19640" activeTab="2" xr2:uid="{E34F97B0-F1C8-E84E-8C54-DB5E482818BA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19640" activeTab="3" xr2:uid="{E34F97B0-F1C8-E84E-8C54-DB5E482818BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Phase 1" sheetId="2" r:id="rId1"/>
     <sheet name="Phase 2" sheetId="3" r:id="rId2"/>
     <sheet name="Cohen's Kappa" sheetId="1" r:id="rId3"/>
+    <sheet name="Identified tools" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="644">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="648">
   <si>
     <t># total</t>
   </si>
@@ -2008,6 +2009,18 @@
   <si>
     <t># include 
 reviewer 1</t>
+  </si>
+  <si>
+    <t>Tool ID</t>
+  </si>
+  <si>
+    <t>CMA</t>
+  </si>
+  <si>
+    <t>contextmap.io</t>
+  </si>
+  <si>
+    <t>Contextmap</t>
   </si>
 </sst>
 </file>
@@ -2138,22 +2151,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -2161,8 +2171,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2176,21 +2185,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
@@ -2531,35 +2526,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32F1D59F-7CBB-AE46-9F18-5E7CF681CC57}">
   <dimension ref="A1:G314"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.6640625" customWidth="1"/>
-    <col min="2" max="5" width="14.1640625" customWidth="1"/>
+    <col min="2" max="3" width="10.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" customWidth="1"/>
+    <col min="5" max="5" width="6.5" customWidth="1"/>
     <col min="6" max="7" width="28" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="43" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="9" t="s">
         <v>635</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>632</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>633</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>634</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="7" t="s">
         <v>639</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>10</v>
       </c>
     </row>
@@ -9486,25 +9485,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="43" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="8" t="s">
         <v>635</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>632</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>633</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>634</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="5" t="s">
         <v>637</v>
       </c>
     </row>
@@ -9564,7 +9563,7 @@
       <c r="F4" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" t="s">
         <v>636</v>
       </c>
     </row>
@@ -9644,7 +9643,7 @@
       <c r="F8" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" t="s">
         <v>638</v>
       </c>
     </row>
@@ -9737,156 +9736,192 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FDA1CBE-66B1-324E-B98D-2E05D797AB75}">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="13"/>
-    <col min="2" max="2" width="6.1640625" style="13" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" style="13" customWidth="1"/>
-    <col min="4" max="7" width="10" style="13" customWidth="1"/>
-    <col min="8" max="8" width="3.5" style="13" customWidth="1"/>
-    <col min="9" max="9" width="4.6640625" style="13" customWidth="1"/>
-    <col min="10" max="10" width="9" style="13" customWidth="1"/>
-    <col min="11" max="11" width="9.5" style="13" customWidth="1"/>
-    <col min="12" max="12" width="10.83203125" style="13"/>
-    <col min="13" max="13" width="1.83203125" style="13" customWidth="1"/>
-    <col min="14" max="14" width="12.83203125" style="13" customWidth="1"/>
-    <col min="15" max="16384" width="10.83203125" style="13"/>
+    <col min="1" max="1" width="10.83203125" style="10"/>
+    <col min="2" max="2" width="6.1640625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" style="10" customWidth="1"/>
+    <col min="4" max="7" width="10" style="10" customWidth="1"/>
+    <col min="8" max="8" width="3.5" style="10" customWidth="1"/>
+    <col min="9" max="9" width="4.6640625" style="10" customWidth="1"/>
+    <col min="10" max="10" width="9" style="10" customWidth="1"/>
+    <col min="11" max="11" width="9.5" style="10" customWidth="1"/>
+    <col min="12" max="12" width="10.83203125" style="10"/>
+    <col min="13" max="13" width="1.83203125" style="10" customWidth="1"/>
+    <col min="14" max="14" width="12.83203125" style="10" customWidth="1"/>
+    <col min="15" max="16384" width="10.83203125" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="29" x14ac:dyDescent="0.2">
-      <c r="A1" s="16"/>
-      <c r="B1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="6" t="s">
+      <c r="A1" s="12"/>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>643</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>642</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>640</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>641</v>
       </c>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6" t="s">
+      <c r="H1" s="5"/>
+      <c r="I1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="6"/>
-      <c r="N1" s="21" t="s">
+      <c r="M1" s="5"/>
+      <c r="N1" s="17" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="1">
         <v>313</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="1">
         <v>310</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="1">
         <v>10</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="1">
         <v>9</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="1">
         <f>B2-D2</f>
         <v>303</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="1">
         <f>B2-E2</f>
         <v>304</v>
       </c>
-      <c r="H2" s="14"/>
-      <c r="I2" s="15">
+      <c r="I2" s="11">
         <f t="shared" ref="I2:I3" si="0">C2/B2</f>
         <v>0.99041533546325877</v>
       </c>
-      <c r="J2" s="15">
+      <c r="J2" s="11">
         <f t="shared" ref="J2:J3" si="1">(D2/B2)*(E2/B2)</f>
         <v>9.1865794281864664E-4</v>
       </c>
-      <c r="K2" s="15">
+      <c r="K2" s="11">
         <f t="shared" ref="K2:K3" si="2">(F2/B2)*(G2/B2)</f>
         <v>0.94021578254345761</v>
       </c>
-      <c r="L2" s="15">
+      <c r="L2" s="11">
         <f t="shared" ref="L2:L3" si="3">J2+K2</f>
         <v>0.94113444048627626</v>
       </c>
-      <c r="M2" s="15"/>
-      <c r="N2" s="22">
+      <c r="M2" s="11"/>
+      <c r="N2" s="18">
         <f t="shared" ref="N2:N3" si="4">(I2-L2)/(1-L2)</f>
         <v>0.8371770417894917</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>10</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>10</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>1</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>1</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <f>B3-D3</f>
         <v>9</v>
       </c>
-      <c r="G3" s="5">
-        <f t="shared" ref="G2:G3" si="5">B3-E3</f>
+      <c r="G3" s="4">
+        <f t="shared" ref="G3" si="5">B3-E3</f>
         <v>9</v>
       </c>
-      <c r="H3" s="19"/>
-      <c r="I3" s="20">
+      <c r="H3" s="15"/>
+      <c r="I3" s="16">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="J3" s="20">
+      <c r="J3" s="16">
         <f t="shared" si="1"/>
         <v>1.0000000000000002E-2</v>
       </c>
-      <c r="K3" s="20">
+      <c r="K3" s="16">
         <f t="shared" si="2"/>
         <v>0.81</v>
       </c>
-      <c r="L3" s="20">
+      <c r="L3" s="16">
         <f t="shared" si="3"/>
         <v>0.82000000000000006</v>
       </c>
-      <c r="M3" s="20"/>
-      <c r="N3" s="23">
+      <c r="M3" s="16"/>
+      <c r="N3" s="19">
         <f t="shared" si="4"/>
         <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FD80C6C-1B26-0342-8319-C896CC47EC38}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>644</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>637</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>645</v>
+      </c>
+      <c r="B2" t="s">
+        <v>647</v>
+      </c>
+      <c r="C2" t="s">
+        <v>646</v>
       </c>
     </row>
   </sheetData>

</xml_diff>